<commit_message>
Add DALYs to TB framework
</commit_message>
<xml_diff>
--- a/atomica/library/tb_framework.xlsx
+++ b/atomica/library/tb_framework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8886B6A9-9027-4DBC-B567-C000E0303278}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E20BFC-0249-4DB2-80D1-8F627124F485}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -866,6 +866,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="A177" authorId="1" shapeId="0" xr:uid="{1F8AAE65-558B-4A5E-B0CD-0E894BC320EB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the rate at which YLDs are being accumulated - integrate over time to get the number of YLDs</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -908,7 +921,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="825">
   <si>
     <t>Name</t>
   </si>
@@ -3329,13 +3342,67 @@
   </si>
   <si>
     <t>spdd:spdt</t>
+  </si>
+  <si>
+    <t>sh_dalys</t>
+  </si>
+  <si>
+    <t>DALYs</t>
+  </si>
+  <si>
+    <t>life_expectancy</t>
+  </si>
+  <si>
+    <t>Estimated number of years of life remaining</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>YLD weighting for untreated TB</t>
+  </si>
+  <si>
+    <t>treated_yld_weight</t>
+  </si>
+  <si>
+    <t>untreated_yld_weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YLD weighting for TB under treatment </t>
+  </si>
+  <si>
+    <t>untreated_yld_weight*(spdu+spdd+spmu+spmd+spxu+spxd+sndu+sndd+snmu+snmd+snxu+snxd)+treated_yld_weight*(spdt+spmt+spxt+sndt+snmt+snxt)</t>
+  </si>
+  <si>
+    <t>life_expectancy*:ddis</t>
+  </si>
+  <si>
+    <t>Number of people</t>
+  </si>
+  <si>
+    <t>yld_rate</t>
+  </si>
+  <si>
+    <t>yll_rate</t>
+  </si>
+  <si>
+    <t>daly_rate</t>
+  </si>
+  <si>
+    <t>YLL rate</t>
+  </si>
+  <si>
+    <t>YLD rate</t>
+  </si>
+  <si>
+    <t>yll_rate + yld_rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3385,6 +3452,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4169,7 +4242,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4261,8 +4334,12 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -4290,8 +4367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6445,8 +6522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8103,19 +8180,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:L176"/>
+  <dimension ref="A1:L180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
+      <selection pane="topRight" activeCell="G181" sqref="G181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="21" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="25" bestFit="1" customWidth="1"/>
@@ -8124,9 +8201,9 @@
     <col min="9" max="9" width="24.7109375" style="37" customWidth="1"/>
     <col min="10" max="10" width="13" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="25" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="25"/>
+    <col min="12" max="12" width="14.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="25" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -12928,19 +13005,113 @@
       <c r="K173" s="6"/>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E174" s="6"/>
+      <c r="C174" s="1"/>
       <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
       <c r="I174" s="36"/>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A175" s="4" t="s">
+        <v>814</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D175" s="6">
+        <v>1</v>
+      </c>
       <c r="E175" s="6"/>
       <c r="F175" s="6"/>
       <c r="I175" s="36"/>
+      <c r="J175" s="19" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176" s="4" t="s">
+        <v>813</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="D176" s="6">
+        <v>1</v>
+      </c>
       <c r="E176" s="6"/>
       <c r="F176" s="6"/>
       <c r="I176" s="36"/>
+      <c r="J176" s="19" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" s="4" t="s">
+        <v>819</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C177" s="25" t="s">
+        <v>818</v>
+      </c>
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" t="s">
+        <v>816</v>
+      </c>
+      <c r="I177" s="36"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="D178" s="6">
+        <v>30</v>
+      </c>
+      <c r="E178" s="6"/>
+      <c r="F178" s="6"/>
+      <c r="I178" s="36"/>
+      <c r="J178" s="19" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C179" s="25" t="s">
+        <v>818</v>
+      </c>
+      <c r="E179" s="6"/>
+      <c r="F179" s="6"/>
+      <c r="G179" s="25" t="s">
+        <v>817</v>
+      </c>
+      <c r="I179" s="36"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>821</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="C180" s="25" t="s">
+        <v>818</v>
+      </c>
+      <c r="G180" s="25" t="s">
+        <v>824</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H128:H145 H148:H1048576 H67:H125 H1:H65">
@@ -12963,8 +13134,8 @@
       <formula>NOT(ISERROR(SEARCH("y",H66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I174:I176" xr:uid="{00000000-0002-0000-0600-000000000000}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I174:I179" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H2:H173" xr:uid="{00000000-0002-0000-0600-000001000000}">
@@ -12972,8 +13143,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Switch to single disutility weight
</commit_message>
<xml_diff>
--- a/atomica/library/tb_framework.xlsx
+++ b/atomica/library/tb_framework.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E20BFC-0249-4DB2-80D1-8F627124F485}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="468" windowWidth="16098" windowHeight="9660" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <sheet name="Plots" sheetId="9" r:id="rId9"/>
     <sheet name="#ignore extra plots" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>None</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,13 +86,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>None</author>
     <author>Romesh</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -228,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
+    <comment ref="J1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -327,13 +326,13 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>None</author>
     <author>Romesh</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -359,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -386,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -413,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -427,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -441,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -484,7 +483,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -504,7 +503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -520,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000A000000}">
+    <comment ref="J1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -539,12 +538,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>None</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -569,7 +568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -595,7 +594,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -614,14 +613,14 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>None</author>
     <author>Romesh</author>
     <author>Rowan</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -644,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -668,7 +667,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -682,7 +681,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -696,7 +695,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -710,7 +709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -724,7 +723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -738,7 +737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -756,7 +755,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000009000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -771,7 +770,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000A000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -791,7 +790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000B000000}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -807,7 +806,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000C000000}">
+    <comment ref="L1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -821,7 +820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G49" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000D000000}">
+    <comment ref="G49" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -836,7 +835,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B57" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000E000000}">
+    <comment ref="B57" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -851,7 +850,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D93" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000F000000}">
+    <comment ref="D93" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -866,7 +865,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A177" authorId="1" shapeId="0" xr:uid="{1F8AAE65-558B-4A5E-B0CD-0E894BC320EB}">
+    <comment ref="A176" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -884,12 +883,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>None</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -921,7 +920,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="823">
   <si>
     <t>Name</t>
   </si>
@@ -3359,21 +3358,6 @@
     <t>years</t>
   </si>
   <si>
-    <t>YLD weighting for untreated TB</t>
-  </si>
-  <si>
-    <t>treated_yld_weight</t>
-  </si>
-  <si>
-    <t>untreated_yld_weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YLD weighting for TB under treatment </t>
-  </si>
-  <si>
-    <t>untreated_yld_weight*(spdu+spdd+spmu+spmd+spxu+spxd+sndu+sndd+snmu+snmd+snxu+snxd)+treated_yld_weight*(spdt+spmt+spxt+sndt+snmt+snxt)</t>
-  </si>
-  <si>
     <t>life_expectancy*:ddis</t>
   </si>
   <si>
@@ -3396,12 +3380,21 @@
   </si>
   <si>
     <t>yll_rate + yld_rate</t>
+  </si>
+  <si>
+    <t>disutility_weight</t>
+  </si>
+  <si>
+    <t>Disutility weight for active TB</t>
+  </si>
+  <si>
+    <t>disutility_weight*(spdu+spdd+spmu+spmd+spxu+spxd+sndu+sndd+snmu+snmd+snxu+snxd+spdt+spmt+spxt+sndt+snmt+snxt)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3613,7 +3606,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutral 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Neutral 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -3734,23 +3727,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3786,23 +3762,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3978,16 +3937,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3995,7 +3954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -4009,21 +3968,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="65" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.26171875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.15625" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>784</v>
       </c>
@@ -4034,7 +3993,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>786</v>
       </c>
@@ -4045,7 +4004,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>788</v>
       </c>
@@ -4056,7 +4015,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>790</v>
       </c>
@@ -4067,7 +4026,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>792</v>
       </c>
@@ -4078,7 +4037,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>794</v>
       </c>
@@ -4089,7 +4048,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>796</v>
       </c>
@@ -4100,7 +4059,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>798</v>
       </c>
@@ -4111,7 +4070,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>800</v>
       </c>
@@ -4122,7 +4081,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>802</v>
       </c>
@@ -4133,7 +4092,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>802</v>
       </c>
@@ -4144,7 +4103,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>804</v>
       </c>
@@ -4155,7 +4114,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>805</v>
       </c>
@@ -4166,7 +4125,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -4177,7 +4136,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -4188,7 +4147,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -4199,7 +4158,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>92</v>
       </c>
@@ -4210,7 +4169,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -4221,7 +4180,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -4238,22 +4197,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="25" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="25.68359375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="34.26171875" style="25" customWidth="1"/>
     <col min="3" max="3" width="9" style="25" customWidth="1"/>
     <col min="4" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4261,7 +4220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -4269,7 +4228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -4277,7 +4236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -4285,7 +4244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -4293,7 +4252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -4301,7 +4260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
@@ -4309,7 +4268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -4317,7 +4276,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
@@ -4325,7 +4284,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
@@ -4333,7 +4292,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
         <v>807</v>
       </c>
@@ -4341,19 +4300,19 @@
         <v>808</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
     </row>
@@ -4364,28 +4323,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26171875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.68359375" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.41796875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26171875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.68359375" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26171875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.15625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="94" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -4417,7 +4376,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="34" t="s">
         <v>34</v>
       </c>
@@ -4445,7 +4404,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -4466,7 +4425,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -4487,7 +4446,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -4508,7 +4467,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4529,7 +4488,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -4550,7 +4509,7 @@
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -4571,7 +4530,7 @@
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -4592,7 +4551,7 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -4613,7 +4572,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="12" t="s">
         <v>55</v>
       </c>
@@ -4636,7 +4595,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -4657,7 +4616,7 @@
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -4678,7 +4637,7 @@
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -4699,7 +4658,7 @@
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -4720,7 +4679,7 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -4741,7 +4700,7 @@
       </c>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -4762,7 +4721,7 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -4783,7 +4742,7 @@
       </c>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -4804,7 +4763,7 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -4825,7 +4784,7 @@
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -4846,7 +4805,7 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -4867,7 +4826,7 @@
       </c>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -4888,7 +4847,7 @@
       </c>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -4909,7 +4868,7 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -4930,7 +4889,7 @@
       </c>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -4951,7 +4910,7 @@
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -4972,7 +4931,7 @@
       </c>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -4993,7 +4952,7 @@
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -5014,7 +4973,7 @@
       </c>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>93</v>
       </c>
@@ -5035,7 +4994,7 @@
       </c>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -5056,7 +5015,7 @@
       </c>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -5077,7 +5036,7 @@
       </c>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -5098,7 +5057,7 @@
       </c>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -5119,7 +5078,7 @@
       </c>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -5140,7 +5099,7 @@
       </c>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -5161,7 +5120,7 @@
       </c>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>107</v>
       </c>
@@ -5182,7 +5141,7 @@
       </c>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -5203,7 +5162,7 @@
       </c>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -5224,7 +5183,7 @@
       </c>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -5245,7 +5204,7 @@
       </c>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="12" t="s">
         <v>115</v>
       </c>
@@ -5268,7 +5227,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>117</v>
       </c>
@@ -5289,7 +5248,7 @@
       </c>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -5310,7 +5269,7 @@
       </c>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="12" t="s">
         <v>121</v>
       </c>
@@ -5333,7 +5292,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>123</v>
       </c>
@@ -5354,7 +5313,7 @@
       </c>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -5375,7 +5334,7 @@
       </c>
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>127</v>
       </c>
@@ -5396,24 +5355,24 @@
       </c>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G51" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:E47" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:E47">
       <formula1>"n,y"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G3:G51" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G3:G51">
       <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5424,7 +5383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5432,60 +5391,60 @@
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.26171875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.26171875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.41796875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.15625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26171875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.15625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.26171875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.578125" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="11.15625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.578125" style="6" customWidth="1"/>
     <col min="22" max="22" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" style="6" customWidth="1"/>
+    <col min="23" max="23" width="9.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.41796875" style="6" customWidth="1"/>
     <col min="28" max="28" width="5" style="6" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="6" style="6" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.42578125" style="6" customWidth="1"/>
-    <col min="33" max="33" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.41796875" style="6" customWidth="1"/>
+    <col min="33" max="33" width="6.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.41796875" style="6" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8" style="6" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="8" style="6" customWidth="1"/>
-    <col min="37" max="37" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.42578125" style="6" customWidth="1"/>
-    <col min="41" max="41" width="11.85546875" style="6" customWidth="1"/>
+    <col min="37" max="37" width="5.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.41796875" style="6" customWidth="1"/>
+    <col min="41" max="41" width="11.83984375" style="6" customWidth="1"/>
     <col min="42" max="42" width="3" style="6" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.15625" style="10" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.83984375" style="6" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="9" style="6" customWidth="1"/>
     <col min="49" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="34" t="s">
         <v>34</v>
       </c>
@@ -5629,7 +5588,7 @@
       <c r="AX1" s="2"/>
       <c r="AY1" s="2"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="34" t="s">
         <v>34</v>
       </c>
@@ -5736,7 +5695,7 @@
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -5754,7 +5713,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -5769,7 +5728,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -5790,7 +5749,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
@@ -5806,7 +5765,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8" t="s">
         <v>47</v>
       </c>
@@ -5819,7 +5778,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -5837,7 +5796,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -5852,7 +5811,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
         <v>53</v>
       </c>
@@ -5865,7 +5824,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -5880,7 +5839,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
@@ -5902,7 +5861,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>59</v>
       </c>
@@ -5917,7 +5876,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
@@ -5929,7 +5888,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>63</v>
       </c>
@@ -5944,7 +5903,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -5965,7 +5924,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
@@ -5986,7 +5945,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
@@ -6001,7 +5960,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="8" t="s">
         <v>71</v>
       </c>
@@ -6022,7 +5981,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
         <v>73</v>
       </c>
@@ -6043,7 +6002,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
@@ -6064,7 +6023,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>77</v>
       </c>
@@ -6080,7 +6039,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="8" t="s">
         <v>79</v>
       </c>
@@ -6101,7 +6060,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>81</v>
       </c>
@@ -6123,7 +6082,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>83</v>
       </c>
@@ -6144,7 +6103,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>85</v>
       </c>
@@ -6160,7 +6119,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="8" t="s">
         <v>87</v>
       </c>
@@ -6178,7 +6137,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -6193,7 +6152,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
         <v>91</v>
       </c>
@@ -6214,7 +6173,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
         <v>93</v>
       </c>
@@ -6235,7 +6194,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
@@ -6251,7 +6210,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="8" t="s">
         <v>97</v>
       </c>
@@ -6272,7 +6231,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
         <v>99</v>
       </c>
@@ -6293,7 +6252,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
         <v>101</v>
       </c>
@@ -6314,7 +6273,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
         <v>103</v>
       </c>
@@ -6330,7 +6289,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="8" t="s">
         <v>105</v>
       </c>
@@ -6351,7 +6310,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
         <v>107</v>
       </c>
@@ -6372,7 +6331,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
         <v>109</v>
       </c>
@@ -6393,7 +6352,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -6409,7 +6368,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="8" t="s">
         <v>113</v>
       </c>
@@ -6427,7 +6386,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2" t="s">
         <v>115</v>
       </c>
@@ -6445,7 +6404,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2" t="s">
         <v>117</v>
       </c>
@@ -6454,7 +6413,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="8" t="s">
         <v>119</v>
       </c>
@@ -6463,7 +6422,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="8" t="s">
         <v>121</v>
       </c>
@@ -6478,37 +6437,37 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
     </row>
@@ -6519,32 +6478,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.68359375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.68359375" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.41796875" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" style="25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="25" customWidth="1"/>
     <col min="11" max="11" width="50" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53.68359375" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="25" customWidth="1"/>
     <col min="14" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -6578,7 +6537,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>250</v>
       </c>
@@ -6601,7 +6560,7 @@
       <c r="I2" s="6"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>253</v>
       </c>
@@ -6624,7 +6583,7 @@
       <c r="I3" s="6"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>256</v>
       </c>
@@ -6646,7 +6605,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>259</v>
       </c>
@@ -6669,7 +6628,7 @@
       <c r="I5" s="6"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>262</v>
       </c>
@@ -6692,7 +6651,7 @@
       <c r="I6" s="6"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>265</v>
       </c>
@@ -6715,7 +6674,7 @@
       <c r="I7" s="6"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="24" t="s">
         <v>268</v>
       </c>
@@ -6739,7 +6698,7 @@
       <c r="K8" s="24"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="24" t="s">
         <v>271</v>
       </c>
@@ -6763,7 +6722,7 @@
       <c r="K9" s="24"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="24" t="s">
         <v>274</v>
       </c>
@@ -6787,7 +6746,7 @@
       <c r="K10" s="24"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="24" t="s">
         <v>277</v>
       </c>
@@ -6811,7 +6770,7 @@
       <c r="K11" s="24"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="24" t="s">
         <v>280</v>
       </c>
@@ -6835,7 +6794,7 @@
       <c r="K12" s="24"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="24" t="s">
         <v>283</v>
       </c>
@@ -6859,7 +6818,7 @@
       <c r="K13" s="24"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="24" t="s">
         <v>286</v>
       </c>
@@ -6879,7 +6838,7 @@
       <c r="K14" s="24"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="24" t="s">
         <v>289</v>
       </c>
@@ -6898,7 +6857,7 @@
       <c r="I15" s="6"/>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="24" t="s">
         <v>292</v>
       </c>
@@ -6922,7 +6881,7 @@
       <c r="K16" s="24"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="24" t="s">
         <v>295</v>
       </c>
@@ -6946,7 +6905,7 @@
       <c r="K17" s="24"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="24" t="s">
         <v>298</v>
       </c>
@@ -6970,7 +6929,7 @@
       <c r="K18" s="24"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="24" t="s">
         <v>301</v>
       </c>
@@ -6994,7 +6953,7 @@
       <c r="K19" s="24"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="24" t="s">
         <v>304</v>
       </c>
@@ -7018,7 +6977,7 @@
       <c r="K20" s="24"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="24" t="s">
         <v>307</v>
       </c>
@@ -7042,7 +7001,7 @@
       <c r="K21" s="24"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="24" t="s">
         <v>310</v>
       </c>
@@ -7065,7 +7024,7 @@
       <c r="I22" s="6"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="24" t="s">
         <v>313</v>
       </c>
@@ -7088,7 +7047,7 @@
       <c r="I23" s="6"/>
       <c r="K23" s="24"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="24" t="s">
         <v>316</v>
       </c>
@@ -7107,7 +7066,7 @@
       <c r="I24" s="6"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="24" t="s">
         <v>319</v>
       </c>
@@ -7126,7 +7085,7 @@
       <c r="I25" s="6"/>
       <c r="K25" s="24"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="24" t="s">
         <v>322</v>
       </c>
@@ -7145,7 +7104,7 @@
       <c r="I26" s="6"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="24" t="s">
         <v>325</v>
       </c>
@@ -7164,7 +7123,7 @@
       <c r="I27" s="6"/>
       <c r="K27" s="24"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="24" t="s">
         <v>328</v>
       </c>
@@ -7187,7 +7146,7 @@
       <c r="I28" s="6"/>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="24" t="s">
         <v>331</v>
       </c>
@@ -7206,7 +7165,7 @@
       <c r="I29" s="6"/>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="24" t="s">
         <v>334</v>
       </c>
@@ -7229,7 +7188,7 @@
       <c r="I30" s="6"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="24" t="s">
         <v>337</v>
       </c>
@@ -7249,7 +7208,7 @@
       <c r="K31" s="24"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="24" t="s">
         <v>340</v>
       </c>
@@ -7269,7 +7228,7 @@
       <c r="K32" s="24"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="24" t="s">
         <v>343</v>
       </c>
@@ -7289,7 +7248,7 @@
       <c r="K33" s="24"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="24" t="s">
         <v>346</v>
       </c>
@@ -7309,7 +7268,7 @@
       <c r="K34" s="24"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="24" t="s">
         <v>349</v>
       </c>
@@ -7329,7 +7288,7 @@
       <c r="K35" s="24"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="24" t="s">
         <v>352</v>
       </c>
@@ -7349,7 +7308,7 @@
       <c r="K36" s="24"/>
       <c r="L36" s="4"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="24" t="s">
         <v>355</v>
       </c>
@@ -7372,7 +7331,7 @@
       <c r="K37" s="24"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="24" t="s">
         <v>357</v>
       </c>
@@ -7395,7 +7354,7 @@
       <c r="K38" s="24"/>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="24" t="s">
         <v>359</v>
       </c>
@@ -7418,7 +7377,7 @@
       <c r="K39" s="24"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="24" t="s">
         <v>361</v>
       </c>
@@ -7441,7 +7400,7 @@
       <c r="K40" s="24"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="24" t="s">
         <v>363</v>
       </c>
@@ -7464,7 +7423,7 @@
       <c r="K41" s="24"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="24" t="s">
         <v>365</v>
       </c>
@@ -7487,7 +7446,7 @@
       <c r="K42" s="24"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="24" t="s">
         <v>367</v>
       </c>
@@ -7510,7 +7469,7 @@
       <c r="K43" s="24"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="24" t="s">
         <v>369</v>
       </c>
@@ -7533,7 +7492,7 @@
       <c r="K44" s="24"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="24" t="s">
         <v>371</v>
       </c>
@@ -7556,7 +7515,7 @@
       <c r="K45" s="24"/>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="24" t="s">
         <v>373</v>
       </c>
@@ -7579,7 +7538,7 @@
       <c r="K46" s="24"/>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="24" t="s">
         <v>375</v>
       </c>
@@ -7602,7 +7561,7 @@
       <c r="K47" s="24"/>
       <c r="L47" s="4"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="24" t="s">
         <v>377</v>
       </c>
@@ -7625,7 +7584,7 @@
       <c r="K48" s="24"/>
       <c r="L48" s="4"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="24" t="s">
         <v>379</v>
       </c>
@@ -7648,7 +7607,7 @@
       <c r="K49" s="24"/>
       <c r="L49" s="4"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="24" t="s">
         <v>381</v>
       </c>
@@ -7671,7 +7630,7 @@
       <c r="K50" s="24"/>
       <c r="L50" s="4"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="24" t="s">
         <v>383</v>
       </c>
@@ -7694,7 +7653,7 @@
       <c r="K51" s="24"/>
       <c r="L51" s="4"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="24" t="s">
         <v>385</v>
       </c>
@@ -7717,7 +7676,7 @@
       <c r="K52" s="24"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="24" t="s">
         <v>387</v>
       </c>
@@ -7742,7 +7701,7 @@
       <c r="K53" s="24"/>
       <c r="L53" s="4"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="24" t="s">
         <v>389</v>
       </c>
@@ -7765,7 +7724,7 @@
       <c r="K54" s="24"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="24" t="s">
         <v>391</v>
       </c>
@@ -7788,7 +7747,7 @@
       <c r="K55" s="24"/>
       <c r="L55" s="4"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="24" t="s">
         <v>393</v>
       </c>
@@ -7813,7 +7772,7 @@
       <c r="K56" s="24"/>
       <c r="L56" s="4"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="24" t="s">
         <v>395</v>
       </c>
@@ -7837,7 +7796,7 @@
       <c r="K57" s="24"/>
       <c r="L57" s="4"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="24" t="s">
         <v>398</v>
       </c>
@@ -7861,7 +7820,7 @@
       <c r="K58" s="24"/>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="24" t="s">
         <v>401</v>
       </c>
@@ -7885,7 +7844,7 @@
       <c r="K59" s="24"/>
       <c r="L59" s="4"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="24" t="s">
         <v>404</v>
       </c>
@@ -7904,7 +7863,7 @@
       <c r="I60" s="6"/>
       <c r="K60" s="24"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="24" t="s">
         <v>407</v>
       </c>
@@ -7923,7 +7882,7 @@
       <c r="I61" s="6"/>
       <c r="K61" s="24"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="24" t="s">
         <v>410</v>
       </c>
@@ -7942,7 +7901,7 @@
       <c r="I62" s="6"/>
       <c r="K62" s="24"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="24" t="s">
         <v>413</v>
       </c>
@@ -7966,7 +7925,7 @@
       <c r="K63" s="24"/>
       <c r="L63" s="4"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="24" t="s">
         <v>416</v>
       </c>
@@ -7990,7 +7949,7 @@
       <c r="K64" s="24"/>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="24" t="s">
         <v>419</v>
       </c>
@@ -8014,7 +7973,7 @@
       <c r="K65" s="24"/>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="24" t="s">
         <v>422</v>
       </c>
@@ -8034,7 +7993,7 @@
       <c r="K66" s="24"/>
       <c r="L66" s="4"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="24" t="s">
         <v>425</v>
       </c>
@@ -8057,7 +8016,7 @@
       <c r="I67" s="6"/>
       <c r="K67" s="24"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>427</v>
       </c>
@@ -8079,7 +8038,7 @@
       <c r="I68" s="6"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="24" t="s">
         <v>429</v>
       </c>
@@ -8101,30 +8060,30 @@
       <c r="K69" s="24"/>
       <c r="L69" s="4"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="G76" s="6"/>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G76" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G76">
       <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8134,23 +8093,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.68359375" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="25" customWidth="1"/>
     <col min="5" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -8161,7 +8120,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>431</v>
       </c>
@@ -8179,34 +8138,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:L180"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="G181" sqref="G181"/>
+      <selection pane="topRight" activeCell="G176" sqref="G176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="21" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.15625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.68359375" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83984375" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="85.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="85.26171875" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="25" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="37" customWidth="1"/>
+    <col min="9" max="9" width="24.68359375" style="37" customWidth="1"/>
     <col min="10" max="10" width="13" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.26171875" style="25" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="25" customWidth="1"/>
     <col min="14" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -8244,7 +8203,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>438</v>
       </c>
@@ -8271,7 +8230,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="18" t="s">
         <v>442</v>
       </c>
@@ -8298,7 +8257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="18" t="s">
         <v>444</v>
       </c>
@@ -8328,7 +8287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="18" t="s">
         <v>446</v>
       </c>
@@ -8358,7 +8317,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="18" t="s">
         <v>448</v>
       </c>
@@ -8387,7 +8346,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="19" t="s">
         <v>450</v>
       </c>
@@ -8416,7 +8375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="19" t="s">
         <v>452</v>
       </c>
@@ -8445,7 +8404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="19" t="s">
         <v>454</v>
       </c>
@@ -8474,7 +8433,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
         <v>177</v>
       </c>
@@ -8503,7 +8462,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>178</v>
       </c>
@@ -8532,7 +8491,7 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4" t="s">
         <v>179</v>
       </c>
@@ -8561,7 +8520,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
         <v>180</v>
       </c>
@@ -8590,7 +8549,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
         <v>181</v>
       </c>
@@ -8619,7 +8578,7 @@
       </c>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
         <v>211</v>
       </c>
@@ -8648,7 +8607,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
         <v>212</v>
       </c>
@@ -8677,7 +8636,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
         <v>213</v>
       </c>
@@ -8706,7 +8665,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
         <v>465</v>
       </c>
@@ -8733,7 +8692,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>468</v>
       </c>
@@ -8758,7 +8717,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
         <v>470</v>
       </c>
@@ -8783,7 +8742,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
         <v>472</v>
       </c>
@@ -8810,7 +8769,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4" t="s">
         <v>474</v>
       </c>
@@ -8835,7 +8794,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4" t="s">
         <v>476</v>
       </c>
@@ -8860,7 +8819,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4" t="s">
         <v>478</v>
       </c>
@@ -8885,7 +8844,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="19" t="s">
         <v>131</v>
       </c>
@@ -8915,7 +8874,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="19" t="s">
         <v>132</v>
       </c>
@@ -8945,7 +8904,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="19" t="s">
         <v>133</v>
       </c>
@@ -8975,7 +8934,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="19" t="s">
         <v>134</v>
       </c>
@@ -9005,7 +8964,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="19" t="s">
         <v>136</v>
       </c>
@@ -9035,7 +8994,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="19" t="s">
         <v>137</v>
       </c>
@@ -9065,7 +9024,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="19" t="s">
         <v>138</v>
       </c>
@@ -9095,7 +9054,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="19" t="s">
         <v>139</v>
       </c>
@@ -9125,7 +9084,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="19" t="s">
         <v>140</v>
       </c>
@@ -9155,7 +9114,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="19" t="s">
         <v>141</v>
       </c>
@@ -9185,7 +9144,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="19" t="s">
         <v>142</v>
       </c>
@@ -9215,7 +9174,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="19" t="s">
         <v>143</v>
       </c>
@@ -9245,7 +9204,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="19" t="s">
         <v>144</v>
       </c>
@@ -9275,7 +9234,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="19" t="s">
         <v>145</v>
       </c>
@@ -9305,7 +9264,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="19" t="s">
         <v>146</v>
       </c>
@@ -9335,7 +9294,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="19" t="s">
         <v>147</v>
       </c>
@@ -9365,7 +9324,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="19" t="s">
         <v>148</v>
       </c>
@@ -9395,7 +9354,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="19" t="s">
         <v>149</v>
       </c>
@@ -9425,7 +9384,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="19" t="s">
         <v>150</v>
       </c>
@@ -9455,7 +9414,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="19" t="s">
         <v>151</v>
       </c>
@@ -9485,7 +9444,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="19" t="s">
         <v>152</v>
       </c>
@@ -9515,7 +9474,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="19" t="s">
         <v>153</v>
       </c>
@@ -9545,7 +9504,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="19" t="s">
         <v>154</v>
       </c>
@@ -9575,7 +9534,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="19" t="s">
         <v>155</v>
       </c>
@@ -9605,7 +9564,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="19" t="s">
         <v>156</v>
       </c>
@@ -9635,7 +9594,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="19" t="s">
         <v>130</v>
       </c>
@@ -9665,7 +9624,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="19" t="s">
         <v>129</v>
       </c>
@@ -9695,7 +9654,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="19" t="s">
         <v>135</v>
       </c>
@@ -9725,7 +9684,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="6" t="s">
         <v>242</v>
       </c>
@@ -9752,7 +9711,7 @@
       </c>
       <c r="K53" s="6"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="6" t="s">
         <v>159</v>
       </c>
@@ -9779,7 +9738,7 @@
       </c>
       <c r="K54" s="6"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="6" t="s">
         <v>243</v>
       </c>
@@ -9808,7 +9767,7 @@
       </c>
       <c r="K55" s="6"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="6" t="s">
         <v>160</v>
       </c>
@@ -9837,7 +9796,7 @@
       </c>
       <c r="K56" s="6"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="6" t="s">
         <v>157</v>
       </c>
@@ -9861,7 +9820,7 @@
       </c>
       <c r="K57" s="6"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="6" t="s">
         <v>543</v>
       </c>
@@ -9887,7 +9846,7 @@
       </c>
       <c r="K58" s="6"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="6" t="s">
         <v>545</v>
       </c>
@@ -9913,7 +9872,7 @@
       </c>
       <c r="K59" s="6"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="6" t="s">
         <v>547</v>
       </c>
@@ -9939,7 +9898,7 @@
       </c>
       <c r="K60" s="6"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="6" t="s">
         <v>550</v>
       </c>
@@ -9967,7 +9926,7 @@
       </c>
       <c r="K61" s="6"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="6" t="s">
         <v>552</v>
       </c>
@@ -9995,7 +9954,7 @@
       </c>
       <c r="K62" s="6"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="6" t="s">
         <v>165</v>
       </c>
@@ -10019,7 +9978,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="6" t="s">
         <v>162</v>
       </c>
@@ -10043,7 +10002,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="6"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="6" t="s">
         <v>173</v>
       </c>
@@ -10067,7 +10026,7 @@
       <c r="J65" s="4"/>
       <c r="K65" s="6"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="6" t="s">
         <v>168</v>
       </c>
@@ -10093,7 +10052,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="26" t="s">
         <v>167</v>
       </c>
@@ -10121,7 +10080,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="26" t="s">
         <v>166</v>
       </c>
@@ -10149,7 +10108,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="26" t="s">
         <v>171</v>
       </c>
@@ -10177,7 +10136,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="26" t="s">
         <v>170</v>
       </c>
@@ -10205,7 +10164,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="6" t="s">
         <v>567</v>
       </c>
@@ -10234,7 +10193,7 @@
       </c>
       <c r="K71" s="6"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="6" t="s">
         <v>569</v>
       </c>
@@ -10263,7 +10222,7 @@
       </c>
       <c r="K72" s="6"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="6" t="s">
         <v>571</v>
       </c>
@@ -10290,7 +10249,7 @@
       </c>
       <c r="K73" s="6"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="4" t="s">
         <v>163</v>
       </c>
@@ -10318,7 +10277,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="4" t="s">
         <v>174</v>
       </c>
@@ -10346,7 +10305,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="4" t="s">
         <v>164</v>
       </c>
@@ -10374,7 +10333,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="4" t="s">
         <v>175</v>
       </c>
@@ -10402,7 +10361,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="4" t="s">
         <v>169</v>
       </c>
@@ -10430,7 +10389,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="4" t="s">
         <v>176</v>
       </c>
@@ -10458,7 +10417,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="4" t="s">
         <v>581</v>
       </c>
@@ -10482,7 +10441,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="4" t="s">
         <v>584</v>
       </c>
@@ -10506,7 +10465,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="4" t="s">
         <v>587</v>
       </c>
@@ -10530,7 +10489,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="4" t="s">
         <v>590</v>
       </c>
@@ -10554,7 +10513,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="4" t="s">
         <v>593</v>
       </c>
@@ -10578,7 +10537,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="4" t="s">
         <v>596</v>
       </c>
@@ -10602,7 +10561,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="4" t="s">
         <v>599</v>
       </c>
@@ -10626,7 +10585,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="4" t="s">
         <v>602</v>
       </c>
@@ -10650,7 +10609,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="4" t="s">
         <v>605</v>
       </c>
@@ -10673,7 +10632,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="6" t="s">
         <v>158</v>
       </c>
@@ -10701,7 +10660,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="6" t="s">
         <v>161</v>
       </c>
@@ -10729,7 +10688,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="6" t="s">
         <v>172</v>
       </c>
@@ -10757,7 +10716,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="6" t="s">
         <v>241</v>
       </c>
@@ -10788,7 +10747,7 @@
       </c>
       <c r="K92" s="6"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="6" t="s">
         <v>240</v>
       </c>
@@ -10816,7 +10775,7 @@
       </c>
       <c r="K93" s="6"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="11" t="s">
         <v>245</v>
       </c>
@@ -10844,7 +10803,7 @@
       </c>
       <c r="K94" s="10"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="10" t="s">
         <v>617</v>
       </c>
@@ -10872,7 +10831,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="11" t="s">
         <v>620</v>
       </c>
@@ -10900,7 +10859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="11" t="s">
         <v>246</v>
       </c>
@@ -10927,7 +10886,7 @@
       </c>
       <c r="K97" s="10"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="10" t="s">
         <v>244</v>
       </c>
@@ -10955,7 +10914,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="99" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="18" t="s">
         <v>182</v>
       </c>
@@ -10979,7 +10938,7 @@
       </c>
       <c r="K99" s="19"/>
     </row>
-    <row r="100" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="18" t="s">
         <v>192</v>
       </c>
@@ -11003,7 +10962,7 @@
       </c>
       <c r="K100" s="19"/>
     </row>
-    <row r="101" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="18" t="s">
         <v>202</v>
       </c>
@@ -11027,7 +10986,7 @@
       </c>
       <c r="K101" s="19"/>
     </row>
-    <row r="102" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="18" t="s">
         <v>214</v>
       </c>
@@ -11051,7 +11010,7 @@
       </c>
       <c r="K102" s="19"/>
     </row>
-    <row r="103" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="18" t="s">
         <v>223</v>
       </c>
@@ -11075,7 +11034,7 @@
       </c>
       <c r="K103" s="19"/>
     </row>
-    <row r="104" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="18" t="s">
         <v>232</v>
       </c>
@@ -11099,7 +11058,7 @@
       </c>
       <c r="K104" s="19"/>
     </row>
-    <row r="105" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="18" t="s">
         <v>632</v>
       </c>
@@ -11124,7 +11083,7 @@
       </c>
       <c r="K105" s="19"/>
     </row>
-    <row r="106" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="18" t="s">
         <v>185</v>
       </c>
@@ -11149,7 +11108,7 @@
       <c r="J106" s="19"/>
       <c r="K106" s="19"/>
     </row>
-    <row r="107" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="18" t="s">
         <v>217</v>
       </c>
@@ -11174,7 +11133,7 @@
       <c r="J107" s="19"/>
       <c r="K107" s="19"/>
     </row>
-    <row r="108" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="18" t="s">
         <v>637</v>
       </c>
@@ -11201,7 +11160,7 @@
       </c>
       <c r="K108" s="19"/>
     </row>
-    <row r="109" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="18" t="s">
         <v>639</v>
       </c>
@@ -11230,7 +11189,7 @@
       </c>
       <c r="K109" s="19"/>
     </row>
-    <row r="110" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="18" t="s">
         <v>641</v>
       </c>
@@ -11259,7 +11218,7 @@
       </c>
       <c r="K110" s="19"/>
     </row>
-    <row r="111" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="18" t="s">
         <v>643</v>
       </c>
@@ -11288,7 +11247,7 @@
       </c>
       <c r="K111" s="19"/>
     </row>
-    <row r="112" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="18" t="s">
         <v>645</v>
       </c>
@@ -11317,7 +11276,7 @@
       </c>
       <c r="K112" s="19"/>
     </row>
-    <row r="113" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="18" t="s">
         <v>647</v>
       </c>
@@ -11346,7 +11305,7 @@
       </c>
       <c r="K113" s="19"/>
     </row>
-    <row r="114" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="18" t="s">
         <v>186</v>
       </c>
@@ -11370,7 +11329,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="29" t="s">
         <v>187</v>
       </c>
@@ -11398,7 +11357,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="29" t="s">
         <v>188</v>
       </c>
@@ -11426,7 +11385,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="117" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="29" t="s">
         <v>189</v>
       </c>
@@ -11454,7 +11413,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="29" t="s">
         <v>190</v>
       </c>
@@ -11482,7 +11441,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="29" t="s">
         <v>191</v>
       </c>
@@ -11510,7 +11469,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="29" t="s">
         <v>218</v>
       </c>
@@ -11538,7 +11497,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="121" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="29" t="s">
         <v>219</v>
       </c>
@@ -11566,7 +11525,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="29" t="s">
         <v>220</v>
       </c>
@@ -11594,7 +11553,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="29" t="s">
         <v>221</v>
       </c>
@@ -11622,7 +11581,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="124" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="29" t="s">
         <v>222</v>
       </c>
@@ -11650,7 +11609,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="125" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="18" t="s">
         <v>661</v>
       </c>
@@ -11675,7 +11634,7 @@
       </c>
       <c r="K125" s="19"/>
     </row>
-    <row r="126" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="18" t="s">
         <v>195</v>
       </c>
@@ -11700,7 +11659,7 @@
       <c r="J126" s="19"/>
       <c r="K126" s="19"/>
     </row>
-    <row r="127" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="18" t="s">
         <v>226</v>
       </c>
@@ -11725,7 +11684,7 @@
       <c r="J127" s="19"/>
       <c r="K127" s="19"/>
     </row>
-    <row r="128" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="18" t="s">
         <v>667</v>
       </c>
@@ -11752,7 +11711,7 @@
       </c>
       <c r="K128" s="19"/>
     </row>
-    <row r="129" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="18" t="s">
         <v>669</v>
       </c>
@@ -11781,7 +11740,7 @@
       </c>
       <c r="K129" s="19"/>
     </row>
-    <row r="130" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="18" t="s">
         <v>671</v>
       </c>
@@ -11810,7 +11769,7 @@
       </c>
       <c r="K130" s="19"/>
     </row>
-    <row r="131" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="18" t="s">
         <v>673</v>
       </c>
@@ -11839,7 +11798,7 @@
       </c>
       <c r="K131" s="19"/>
     </row>
-    <row r="132" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="18" t="s">
         <v>675</v>
       </c>
@@ -11868,7 +11827,7 @@
       </c>
       <c r="K132" s="19"/>
     </row>
-    <row r="133" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="18" t="s">
         <v>677</v>
       </c>
@@ -11897,7 +11856,7 @@
       </c>
       <c r="K133" s="19"/>
     </row>
-    <row r="134" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="18" t="s">
         <v>196</v>
       </c>
@@ -11921,7 +11880,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="135" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="29" t="s">
         <v>197</v>
       </c>
@@ -11949,7 +11908,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="136" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="29" t="s">
         <v>198</v>
       </c>
@@ -11977,7 +11936,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="137" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="29" t="s">
         <v>199</v>
       </c>
@@ -12005,7 +11964,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="138" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="29" t="s">
         <v>200</v>
       </c>
@@ -12033,7 +11992,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="139" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="29" t="s">
         <v>201</v>
       </c>
@@ -12061,7 +12020,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="140" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="29" t="s">
         <v>227</v>
       </c>
@@ -12089,7 +12048,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="141" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="29" t="s">
         <v>228</v>
       </c>
@@ -12117,7 +12076,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="142" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="29" t="s">
         <v>229</v>
       </c>
@@ -12145,7 +12104,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="143" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="29" t="s">
         <v>230</v>
       </c>
@@ -12173,7 +12132,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="144" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="29" t="s">
         <v>231</v>
       </c>
@@ -12201,7 +12160,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="145" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="20" t="s">
         <v>691</v>
       </c>
@@ -12226,7 +12185,7 @@
       </c>
       <c r="K145" s="22"/>
     </row>
-    <row r="146" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="18" t="s">
         <v>205</v>
       </c>
@@ -12251,7 +12210,7 @@
       <c r="J146" s="19"/>
       <c r="K146" s="19"/>
     </row>
-    <row r="147" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="18" t="s">
         <v>235</v>
       </c>
@@ -12276,7 +12235,7 @@
       <c r="J147" s="19"/>
       <c r="K147" s="19"/>
     </row>
-    <row r="148" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="20" t="s">
         <v>697</v>
       </c>
@@ -12303,7 +12262,7 @@
       </c>
       <c r="K148" s="22"/>
     </row>
-    <row r="149" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="20" t="s">
         <v>699</v>
       </c>
@@ -12332,7 +12291,7 @@
       </c>
       <c r="K149" s="22"/>
     </row>
-    <row r="150" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="20" t="s">
         <v>701</v>
       </c>
@@ -12361,7 +12320,7 @@
       </c>
       <c r="K150" s="22"/>
     </row>
-    <row r="151" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="20" t="s">
         <v>703</v>
       </c>
@@ -12390,7 +12349,7 @@
       </c>
       <c r="K151" s="22"/>
     </row>
-    <row r="152" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="20" t="s">
         <v>705</v>
       </c>
@@ -12419,7 +12378,7 @@
       </c>
       <c r="K152" s="22"/>
     </row>
-    <row r="153" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="20" t="s">
         <v>206</v>
       </c>
@@ -12444,7 +12403,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="29" t="s">
         <v>207</v>
       </c>
@@ -12472,7 +12431,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="29" t="s">
         <v>208</v>
       </c>
@@ -12500,7 +12459,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="156" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="29" t="s">
         <v>209</v>
       </c>
@@ -12528,7 +12487,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="157" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="29" t="s">
         <v>210</v>
       </c>
@@ -12556,7 +12515,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="158" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="29" t="s">
         <v>236</v>
       </c>
@@ -12584,7 +12543,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="159" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="29" t="s">
         <v>237</v>
       </c>
@@ -12612,7 +12571,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="160" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="29" t="s">
         <v>238</v>
       </c>
@@ -12640,7 +12599,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="161" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="29" t="s">
         <v>239</v>
       </c>
@@ -12668,7 +12627,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="4" t="s">
         <v>183</v>
       </c>
@@ -12696,7 +12655,7 @@
       </c>
       <c r="K162" s="6"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="4" t="s">
         <v>193</v>
       </c>
@@ -12724,7 +12683,7 @@
       </c>
       <c r="K163" s="6"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="4" t="s">
         <v>203</v>
       </c>
@@ -12752,7 +12711,7 @@
       </c>
       <c r="K164" s="6"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="4" t="s">
         <v>215</v>
       </c>
@@ -12780,7 +12739,7 @@
       </c>
       <c r="K165" s="6"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="4" t="s">
         <v>224</v>
       </c>
@@ -12808,7 +12767,7 @@
       </c>
       <c r="K166" s="6"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="4" t="s">
         <v>233</v>
       </c>
@@ -12836,7 +12795,7 @@
       </c>
       <c r="K167" s="6"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="4" t="s">
         <v>184</v>
       </c>
@@ -12864,7 +12823,7 @@
       </c>
       <c r="K168" s="6"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="4" t="s">
         <v>194</v>
       </c>
@@ -12892,7 +12851,7 @@
       </c>
       <c r="K169" s="6"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="4" t="s">
         <v>204</v>
       </c>
@@ -12920,7 +12879,7 @@
       </c>
       <c r="K170" s="6"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="4" t="s">
         <v>216</v>
       </c>
@@ -12948,7 +12907,7 @@
       </c>
       <c r="K171" s="6"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="4" t="s">
         <v>225</v>
       </c>
@@ -12976,7 +12935,7 @@
       </c>
       <c r="K172" s="6"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="4" t="s">
         <v>234</v>
       </c>
@@ -13004,18 +12963,18 @@
       </c>
       <c r="K173" s="6"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C174" s="1"/>
       <c r="F174" s="6"/>
       <c r="G174" s="6"/>
       <c r="I174" s="36"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="4" t="s">
-        <v>814</v>
+        <v>820</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>812</v>
+        <v>821</v>
       </c>
       <c r="D175" s="6">
         <v>1</v>
@@ -13027,94 +12986,77 @@
         <v>807</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="4" t="s">
+        <v>814</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C176" s="25" t="s">
         <v>813</v>
       </c>
-      <c r="B176" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="D176" s="6">
-        <v>1</v>
-      </c>
+      <c r="D176" s="6"/>
       <c r="E176" s="6"/>
       <c r="F176" s="6"/>
+      <c r="G176" t="s">
+        <v>822</v>
+      </c>
       <c r="I176" s="36"/>
-      <c r="J176" s="19" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="4" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="C177" s="25" t="s">
-        <v>818</v>
-      </c>
-      <c r="D177" s="6"/>
+        <v>810</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="D177" s="6">
+        <v>30</v>
+      </c>
       <c r="E177" s="6"/>
       <c r="F177" s="6"/>
-      <c r="G177" t="s">
-        <v>816</v>
-      </c>
       <c r="I177" s="36"/>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J177" s="19" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="4" t="s">
-        <v>809</v>
+        <v>815</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>810</v>
-      </c>
-      <c r="C178" s="6" t="s">
-        <v>811</v>
-      </c>
-      <c r="D178" s="6">
-        <v>30</v>
+        <v>817</v>
+      </c>
+      <c r="C178" s="25" t="s">
+        <v>813</v>
       </c>
       <c r="E178" s="6"/>
       <c r="F178" s="6"/>
+      <c r="G178" s="25" t="s">
+        <v>812</v>
+      </c>
       <c r="I178" s="36"/>
-      <c r="J178" s="19" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="4" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>822</v>
+        <v>808</v>
       </c>
       <c r="C179" s="25" t="s">
-        <v>818</v>
-      </c>
-      <c r="E179" s="6"/>
-      <c r="F179" s="6"/>
+        <v>813</v>
+      </c>
       <c r="G179" s="25" t="s">
-        <v>817</v>
-      </c>
-      <c r="I179" s="36"/>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A180" s="4" t="s">
-        <v>821</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="C180" s="25" t="s">
-        <v>818</v>
-      </c>
-      <c r="G180" s="25" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H128:H145 H148:H1048576 H67:H125 H1:H65">
+  <conditionalFormatting sqref="H128:H145 H67:H125 H1:H65 H148:H1048576">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",H1)))</formula>
     </cfRule>
@@ -13135,11 +13077,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I174:I179" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H2:H173">
+      <formula1>"n,y"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I174:I178">
       <formula1>"y,n"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H2:H173" xr:uid="{00000000-0002-0000-0600-000001000000}">
-      <formula1>"n,y"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13149,20 +13091,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.83984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83984375" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>729</v>
       </c>
@@ -13170,7 +13112,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>731</v>
       </c>
@@ -13178,7 +13120,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>732</v>
       </c>
@@ -13186,7 +13128,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>733</v>
       </c>
@@ -13194,7 +13136,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>734</v>
       </c>
@@ -13202,7 +13144,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>735</v>
       </c>
@@ -13210,7 +13152,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>732</v>
       </c>
@@ -13218,7 +13160,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>733</v>
       </c>
@@ -13226,7 +13168,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5" t="s">
         <v>738</v>
       </c>
@@ -13235,7 +13177,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>739</v>
       </c>
@@ -13244,7 +13186,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>732</v>
       </c>
@@ -13253,7 +13195,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>733</v>
       </c>
@@ -13262,16 +13204,16 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" s="24"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="4"/>
     </row>
   </sheetData>
@@ -13281,21 +13223,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.15625" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="25" customWidth="1"/>
-    <col min="3" max="3" width="104.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.26171875" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -13309,7 +13251,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>335</v>
       </c>
@@ -13323,7 +13265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>746</v>
       </c>
@@ -13337,7 +13279,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>731</v>
       </c>
@@ -13351,7 +13293,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>747</v>
       </c>
@@ -13365,7 +13307,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>748</v>
       </c>
@@ -13379,7 +13321,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>749</v>
       </c>
@@ -13393,7 +13335,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>750</v>
       </c>
@@ -13407,7 +13349,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>752</v>
       </c>
@@ -13421,7 +13363,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>754</v>
       </c>
@@ -13435,7 +13377,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>755</v>
       </c>
@@ -13449,7 +13391,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>756</v>
       </c>
@@ -13463,7 +13405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>758</v>
       </c>
@@ -13477,7 +13419,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -13491,7 +13433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>760</v>
       </c>
@@ -13505,7 +13447,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>761</v>
       </c>
@@ -13519,7 +13461,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>763</v>
       </c>
@@ -13533,7 +13475,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>764</v>
       </c>
@@ -13547,7 +13489,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>765</v>
       </c>
@@ -13561,7 +13503,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>766</v>
       </c>
@@ -13575,7 +13517,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>768</v>
       </c>
@@ -13589,7 +13531,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>770</v>
       </c>
@@ -13603,7 +13545,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>772</v>
       </c>
@@ -13617,7 +13559,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>774</v>
       </c>
@@ -13631,7 +13573,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>776</v>
       </c>
@@ -13645,7 +13587,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>778</v>
       </c>
@@ -13659,7 +13601,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>780</v>
       </c>
@@ -13673,7 +13615,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>782</v>
       </c>

</xml_diff>

<commit_message>
Add default 0 for WHO diagnosis rate so it isn't mandatory
</commit_message>
<xml_diff>
--- a/atomica/library/tb_framework.xlsx
+++ b/atomica/library/tb_framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -9108,11 +9108,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M285"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B262" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E165" sqref="E165"/>
+      <selection pane="bottomRight" activeCell="E295" sqref="E295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15444,7 +15444,7 @@
         <v>0</v>
       </c>
       <c r="F274" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G274" s="17" t="s">
         <v>1098</v>
@@ -15464,7 +15464,7 @@
         <v>0</v>
       </c>
       <c r="F275" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G275" s="17" t="s">
         <v>1099</v>
@@ -15484,7 +15484,7 @@
         <v>0</v>
       </c>
       <c r="F276" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G276" s="17" t="s">
         <v>1100</v>
@@ -15504,7 +15504,7 @@
         <v>0</v>
       </c>
       <c r="F277" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G277" s="17" t="s">
         <v>1101</v>
@@ -15524,7 +15524,7 @@
         <v>0</v>
       </c>
       <c r="F278" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G278" s="17" t="s">
         <v>1102</v>
@@ -15544,7 +15544,7 @@
         <v>0</v>
       </c>
       <c r="F279" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G279" s="17" t="s">
         <v>1103</v>
@@ -15564,7 +15564,7 @@
         <v>0</v>
       </c>
       <c r="F280" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G280" s="17" t="s">
         <v>1104</v>
@@ -15584,7 +15584,7 @@
         <v>0</v>
       </c>
       <c r="F281" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G281" s="17" t="s">
         <v>1105</v>
@@ -15604,7 +15604,7 @@
         <v>0</v>
       </c>
       <c r="F282" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G282" s="17" t="s">
         <v>1106</v>
@@ -15624,7 +15624,7 @@
         <v>0</v>
       </c>
       <c r="F283" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G283" s="17" t="s">
         <v>1107</v>
@@ -15644,7 +15644,7 @@
         <v>0</v>
       </c>
       <c r="F284" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G284" s="17" t="s">
         <v>1108</v>
@@ -15660,11 +15660,14 @@
       <c r="C285" s="6" t="s">
         <v>440</v>
       </c>
+      <c r="D285" s="24">
+        <v>0</v>
+      </c>
       <c r="E285" s="24">
         <v>0</v>
       </c>
       <c r="F285" s="24">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G285" s="17" t="s">
         <v>1109</v>
@@ -15889,7 +15892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>

</xml_diff>